<commit_message>
Michaels stress inversion technique added
</commit_message>
<xml_diff>
--- a/inst/angelier_data.xlsx
+++ b/inst/angelier_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tstephan\Documents\GitHub\stress.inversion\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tstephan\Documents\GitHub\structr\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EB6E9E-B167-40BD-A327-57C001229476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6388B7DD-2056-4419-A74A-EFE7B88D9EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15800" xr2:uid="{1DCBFD59-08CB-40D3-9FD6-974C440FA5C2}"/>
+    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{1DCBFD59-08CB-40D3-9FD6-974C440FA5C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -219,11 +219,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -237,6 +246,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80732589-1979-4E53-BE38-13E5286AC27D}">
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3"/>
@@ -736,7 +749,7 @@
         <v>16</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s">
         <v>38</v>
@@ -1150,7 +1163,7 @@
         <v>39</v>
       </c>
       <c r="D17">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
         <v>37</v>
@@ -1255,7 +1268,7 @@
         <v>49</v>
       </c>
       <c r="D20">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
@@ -1296,7 +1309,7 @@
         <v>16</v>
       </c>
       <c r="F21">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G21" t="s">
         <v>38</v>
@@ -1734,38 +1747,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:11" s="6" customFormat="1">
+      <c r="A34" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="6">
         <v>70</v>
       </c>
-      <c r="D34">
-        <v>60</v>
-      </c>
-      <c r="E34" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34">
+      <c r="D34" s="6">
+        <v>80</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="6">
         <v>89</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="6">
         <v>58</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="6">
         <v>0</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="6">
         <v>65</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="6">
         <v>1</v>
       </c>
     </row>
@@ -1821,7 +1834,7 @@
         <v>38</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="G36" t="s">
         <v>39</v>
@@ -1850,7 +1863,7 @@
         <v>92</v>
       </c>
       <c r="D37">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E37" t="s">
         <v>16</v>
@@ -1891,7 +1904,7 @@
         <v>16</v>
       </c>
       <c r="F38">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G38" t="s">
         <v>37</v>
@@ -1955,7 +1968,7 @@
         <v>112</v>
       </c>
       <c r="D40">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E40" t="s">
         <v>16</v>
@@ -1990,7 +2003,7 @@
         <v>76</v>
       </c>
       <c r="D41">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E41" t="s">
         <v>16</v>
@@ -2101,7 +2114,7 @@
         <v>39</v>
       </c>
       <c r="F44">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="G44" t="s">
         <v>38</v>
@@ -2451,7 +2464,7 @@
         <v>39</v>
       </c>
       <c r="F54">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="G54" t="s">
         <v>38</v>
@@ -2591,7 +2604,7 @@
         <v>37</v>
       </c>
       <c r="F58">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="G58" t="s">
         <v>16</v>
@@ -2795,7 +2808,7 @@
         <v>30</v>
       </c>
       <c r="D64">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E64" t="s">
         <v>38</v>
@@ -2871,7 +2884,7 @@
         <v>38</v>
       </c>
       <c r="F66">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="G66" t="s">
         <v>39</v>
@@ -2900,13 +2913,13 @@
         <v>25</v>
       </c>
       <c r="D67">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E67" t="s">
         <v>38</v>
       </c>
       <c r="F67">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="G67" t="s">
         <v>16</v>
@@ -2967,31 +2980,19 @@
         <v>16</v>
       </c>
       <c r="C69">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="D69">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E69" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69">
+        <v>88</v>
+      </c>
+      <c r="G69" t="s">
         <v>37</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69" t="s">
-        <v>16</v>
-      </c>
-      <c r="H69">
-        <v>37</v>
-      </c>
-      <c r="I69">
-        <v>14</v>
-      </c>
-      <c r="J69">
-        <v>48</v>
-      </c>
-      <c r="K69">
-        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -3002,31 +3003,31 @@
         <v>16</v>
       </c>
       <c r="C70">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="D70">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E70" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F70">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="G70" t="s">
+        <v>16</v>
+      </c>
+      <c r="H70">
         <v>37</v>
       </c>
-      <c r="H70">
-        <v>50</v>
-      </c>
       <c r="I70">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J70">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K70">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -3037,66 +3038,66 @@
         <v>16</v>
       </c>
       <c r="C71">
+        <v>96</v>
+      </c>
+      <c r="D71">
+        <v>70</v>
+      </c>
+      <c r="E71" t="s">
+        <v>16</v>
+      </c>
+      <c r="F71">
+        <v>72</v>
+      </c>
+      <c r="G71" t="s">
+        <v>37</v>
+      </c>
+      <c r="H71">
+        <v>50</v>
+      </c>
+      <c r="I71">
+        <v>6</v>
+      </c>
+      <c r="J71">
+        <v>57</v>
+      </c>
+      <c r="K71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="6" customFormat="1">
+      <c r="A72" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="6">
         <v>89</v>
       </c>
-      <c r="D71">
+      <c r="D72" s="6">
         <v>71</v>
       </c>
-      <c r="E71" t="s">
-        <v>16</v>
-      </c>
-      <c r="F71">
+      <c r="E72" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72" s="6">
         <v>89</v>
       </c>
-      <c r="G71" t="s">
-        <v>38</v>
-      </c>
-      <c r="H71">
+      <c r="G72" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H72" s="6">
         <v>29</v>
       </c>
-      <c r="I71">
+      <c r="I72" s="6">
         <v>5</v>
       </c>
-      <c r="J71">
+      <c r="J72" s="6">
         <v>43</v>
       </c>
-      <c r="K71">
+      <c r="K72" s="6">
         <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
-      <c r="A72" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C72">
-        <v>70</v>
-      </c>
-      <c r="D72">
-        <v>69</v>
-      </c>
-      <c r="E72" t="s">
-        <v>39</v>
-      </c>
-      <c r="F72">
-        <v>80</v>
-      </c>
-      <c r="G72" t="s">
-        <v>37</v>
-      </c>
-      <c r="H72">
-        <v>46</v>
-      </c>
-      <c r="I72">
-        <v>24</v>
-      </c>
-      <c r="J72">
-        <v>50</v>
-      </c>
-      <c r="K72">
-        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:11">

</xml_diff>